<commit_message>
ya en prod admisiones con log
</commit_message>
<xml_diff>
--- a/newAdmision.xlsx
+++ b/newAdmision.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="60">
   <si>
     <t xml:space="preserve">HOSPITAL GENERAL SAN JUAN DE DIOS </t>
   </si>
@@ -40,18 +40,6 @@
     <t>No. Expediente Clinico</t>
   </si>
   <si>
-    <t>García</t>
-  </si>
-  <si>
-    <t>Figueroa</t>
-  </si>
-  <si>
-    <t>kevin</t>
-  </si>
-  <si>
-    <t>Estuardo</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -70,27 +58,12 @@
     <t>Teléfono</t>
   </si>
   <si>
-    <t>Gutemala</t>
-  </si>
-  <si>
-    <t>47000538</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dirección habitual </t>
   </si>
   <si>
     <t xml:space="preserve">Teléfono </t>
   </si>
   <si>
-    <t xml:space="preserve">9a. ave 4-71 </t>
-  </si>
-  <si>
-    <t>Zona 19 colonia la florida</t>
-  </si>
-  <si>
-    <t>guatemala</t>
-  </si>
-  <si>
     <t>Fecha de nacimiento (Día     Mes     Año )</t>
   </si>
   <si>
@@ -103,12 +76,6 @@
     <t>Sexo</t>
   </si>
   <si>
-    <t>23/11/1992</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 24</t>
-  </si>
-  <si>
     <t>MASCULINO</t>
   </si>
   <si>
@@ -124,16 +91,7 @@
     <t>No. De Cédula</t>
   </si>
   <si>
-    <t>Soltero</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> estudiante </t>
-  </si>
-  <si>
-    <t>guatemalteco</t>
-  </si>
-  <si>
-    <t>2424583430101</t>
+    <t>Casado</t>
   </si>
   <si>
     <t>Nombre del Cónyugue</t>
@@ -148,12 +106,6 @@
     <t xml:space="preserve">Nombre de la Madre: </t>
   </si>
   <si>
-    <t>Manolo García</t>
-  </si>
-  <si>
-    <t>Aura Leticia Figueroa</t>
-  </si>
-  <si>
     <t>En caso de emergencia notificar a :</t>
   </si>
   <si>
@@ -163,9 +115,6 @@
     <t>Dirección</t>
   </si>
   <si>
-    <t xml:space="preserve">madre </t>
-  </si>
-  <si>
     <t xml:space="preserve">Otras Hospitalizaciones </t>
   </si>
   <si>
@@ -188,12 +137,6 @@
   </si>
   <si>
     <t>Dias de estancia</t>
-  </si>
-  <si>
-    <t>11/10/2017</t>
-  </si>
-  <si>
-    <t>12:46pm</t>
   </si>
   <si>
     <t xml:space="preserve">IMPRESIÓN CLINICA DE INGRESO </t>
@@ -1086,173 +1029,173 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K7" s="9"/>
     </row>
     <row r="8" ht="12.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="7" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="10" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="K9" s="10"/>
     </row>
     <row r="10" ht="18" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="7" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="12" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="12" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="I11" s="12"/>
       <c r="J11" s="10" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="K11" s="10"/>
     </row>
     <row r="12" ht="14.25" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="13" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="13" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="I12" s="13"/>
       <c r="J12" s="7" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="12" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="12" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="10" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
@@ -1260,20 +1203,20 @@
     </row>
     <row r="14" ht="21.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="13" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="G14" s="13"/>
       <c r="H14" s="7" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
@@ -1281,14 +1224,14 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="12" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
@@ -1298,14 +1241,14 @@
     </row>
     <row r="16" ht="12" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="13" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
@@ -1315,14 +1258,14 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
       <c r="F17" s="18" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
@@ -1332,14 +1275,14 @@
     </row>
     <row r="18" ht="16.5" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
       <c r="F18" s="22" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
@@ -1349,56 +1292,56 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="24" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="G19" s="24"/>
       <c r="H19" s="24" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="I19" s="24"/>
       <c r="J19" s="9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K19" s="9"/>
     </row>
     <row r="20" ht="17.25" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="13" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="13" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I20" s="13"/>
       <c r="J20" s="7" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="K20" s="7"/>
     </row>
     <row r="21" ht="12.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="25" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="G21" s="25"/>
       <c r="H21" s="25"/>
@@ -1408,14 +1351,14 @@
     </row>
     <row r="22" ht="12.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -1425,39 +1368,39 @@
     </row>
     <row r="23" ht="18" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="28" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="D23" s="28" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="E23" s="28"/>
       <c r="F23" s="18" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="G23" s="29"/>
       <c r="H23" s="30" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="I23" s="30"/>
       <c r="J23" s="31" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="K23" s="31"/>
     </row>
     <row r="24" ht="16.5" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="7" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="13"/>
@@ -1469,7 +1412,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="32" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
@@ -1510,7 +1453,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="B28" s="33"/>
       <c r="C28" s="33"/>
@@ -1521,7 +1464,7 @@
       <c r="H28" s="33"/>
       <c r="I28" s="33"/>
       <c r="J28" s="34" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="K28" s="34"/>
     </row>
@@ -1553,7 +1496,7 @@
     </row>
     <row r="31" ht="21" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="33" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B31" s="33"/>
       <c r="C31" s="33"/>
@@ -1564,7 +1507,7 @@
       <c r="H31" s="33"/>
       <c r="I31" s="33"/>
       <c r="J31" s="40" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="K31" s="40"/>
     </row>
@@ -1609,7 +1552,7 @@
     </row>
     <row r="35" ht="21" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="33" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="B35" s="33"/>
       <c r="C35" s="33"/>
@@ -1620,7 +1563,7 @@
       <c r="H35" s="33"/>
       <c r="I35" s="33"/>
       <c r="J35" s="40" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="K35" s="40"/>
     </row>
@@ -1653,46 +1596,46 @@
     </row>
     <row r="38" ht="24" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="43" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="B38" s="44" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="C38" s="44" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="D38" s="44"/>
       <c r="E38" s="44" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="F38" s="44"/>
       <c r="G38" s="44" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="H38" s="44"/>
       <c r="I38" s="44"/>
       <c r="J38" s="45" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="K38" s="45"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="46"/>
       <c r="B39" s="47" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="C39" s="47" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="D39" s="47"/>
       <c r="E39" s="47"/>
       <c r="F39" s="47" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="G39" s="47"/>
       <c r="H39" s="47"/>
       <c r="I39" s="34" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="J39" s="34"/>
       <c r="K39" s="34"/>
@@ -1712,7 +1655,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="49" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="B41" s="49"/>
       <c r="C41" s="49"/>
@@ -1721,13 +1664,13 @@
       <c r="F41" s="49"/>
       <c r="G41" s="49"/>
       <c r="H41" s="47" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="K41" s="50"/>
     </row>
     <row r="42" ht="15" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="51" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="B42" s="51"/>
       <c r="C42" s="51"/>
@@ -1742,7 +1685,7 @@
     </row>
     <row r="43" ht="18.75" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="52" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="B43" s="52"/>
       <c r="C43" s="52"/>

</xml_diff>

<commit_message>
Emergencia terminada servicio ingresos corriendo ok
</commit_message>
<xml_diff>
--- a/newAdmision.xlsx
+++ b/newAdmision.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="84">
   <si>
     <t xml:space="preserve">HOSPITAL GENERAL SAN JUAN DE DIOS </t>
   </si>
@@ -40,30 +40,60 @@
     <t>No. Expediente Clinico</t>
   </si>
   <si>
+    <t>ENRIQUE</t>
+  </si>
+  <si>
+    <t>JAVIER</t>
+  </si>
+  <si>
+    <t>MATÍAS</t>
+  </si>
+  <si>
+    <t>PABLO</t>
+  </si>
+  <si>
+    <t>2017-209</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dirección actual </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calle o lugar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Municipio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Departamento </t>
+  </si>
+  <si>
+    <t>Teléfono</t>
+  </si>
+  <si>
+    <t>SECTOR 3</t>
+  </si>
+  <si>
+    <t>LOTE 242</t>
+  </si>
+  <si>
+    <t>ASENTAMIENTO UNIDOS POR LA PAZ</t>
+  </si>
+  <si>
+    <t>VILLA NUEVA</t>
+  </si>
+  <si>
+    <t>53262877</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dirección habitual </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teléfono </t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t xml:space="preserve">Dirección actual </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calle o lugar </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Municipio </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Departamento </t>
-  </si>
-  <si>
-    <t>Teléfono</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dirección habitual </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teléfono </t>
-  </si>
-  <si>
     <t>Fecha de nacimiento (Día     Mes     Año )</t>
   </si>
   <si>
@@ -76,6 +106,15 @@
     <t>Sexo</t>
   </si>
   <si>
+    <t>20 NOVIEMBRE 1991</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>COMITANCILLO SAN MARCOS</t>
+  </si>
+  <si>
     <t>MASCULINO</t>
   </si>
   <si>
@@ -91,7 +130,16 @@
     <t>No. De Cédula</t>
   </si>
   <si>
-    <t>Casado</t>
+    <t>Soltero</t>
+  </si>
+  <si>
+    <t>ESTUDIANTE</t>
+  </si>
+  <si>
+    <t>GUATEMALTECA</t>
+  </si>
+  <si>
+    <t>2397590791204</t>
   </si>
   <si>
     <t>Nombre del Cónyugue</t>
@@ -106,6 +154,12 @@
     <t xml:space="preserve">Nombre de la Madre: </t>
   </si>
   <si>
+    <t>FRANCISCO JAVIER MATIAS</t>
+  </si>
+  <si>
+    <t>ANA FLORA PABLO</t>
+  </si>
+  <si>
     <t>En caso de emergencia notificar a :</t>
   </si>
   <si>
@@ -115,6 +169,15 @@
     <t>Dirección</t>
   </si>
   <si>
+    <t>PADRE</t>
+  </si>
+  <si>
+    <t>SAN MARCOS</t>
+  </si>
+  <si>
+    <t>45101607</t>
+  </si>
+  <si>
     <t xml:space="preserve">Otras Hospitalizaciones </t>
   </si>
   <si>
@@ -137,6 +200,15 @@
   </si>
   <si>
     <t>Dias de estancia</t>
+  </si>
+  <si>
+    <t>12 OCTUBRE 2017</t>
+  </si>
+  <si>
+    <t>11:25</t>
+  </si>
+  <si>
+    <t>CLINICA 20</t>
   </si>
   <si>
     <t xml:space="preserve">IMPRESIÓN CLINICA DE INGRESO </t>
@@ -1029,173 +1101,173 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="9" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="K7" s="9"/>
     </row>
     <row r="8" ht="12.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="7" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="9" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="10" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="K9" s="10"/>
     </row>
     <row r="10" ht="18" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="7" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="12" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="12" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="I11" s="12"/>
       <c r="J11" s="10" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="K11" s="10"/>
     </row>
     <row r="12" ht="14.25" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="13" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="13" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="I12" s="13"/>
       <c r="J12" s="7" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="12" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="12" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="10" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
@@ -1203,20 +1275,20 @@
     </row>
     <row r="14" ht="21.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="13" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="G14" s="13"/>
       <c r="H14" s="7" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
@@ -1224,14 +1296,14 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="12" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
@@ -1241,14 +1313,14 @@
     </row>
     <row r="16" ht="12" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="13" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
@@ -1258,14 +1330,14 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
       <c r="F17" s="18" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
@@ -1275,14 +1347,14 @@
     </row>
     <row r="18" ht="16.5" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
       <c r="F18" s="22" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
@@ -1292,56 +1364,56 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="24" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="G19" s="24"/>
       <c r="H19" s="24" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="I19" s="24"/>
       <c r="J19" s="9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="K19" s="9"/>
     </row>
     <row r="20" ht="17.25" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="13" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="13" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="I20" s="13"/>
       <c r="J20" s="7" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="K20" s="7"/>
     </row>
     <row r="21" ht="12.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="25" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="G21" s="25"/>
       <c r="H21" s="25"/>
@@ -1351,14 +1423,14 @@
     </row>
     <row r="22" ht="12.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="3" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -1368,39 +1440,39 @@
     </row>
     <row r="23" ht="18" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="28" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="D23" s="28" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="E23" s="28"/>
       <c r="F23" s="18" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="G23" s="29"/>
       <c r="H23" s="30" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="I23" s="30"/>
       <c r="J23" s="31" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="K23" s="31"/>
     </row>
     <row r="24" ht="16.5" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="7" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="13"/>
@@ -1412,7 +1484,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="32" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
@@ -1453,7 +1525,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="B28" s="33"/>
       <c r="C28" s="33"/>
@@ -1464,7 +1536,7 @@
       <c r="H28" s="33"/>
       <c r="I28" s="33"/>
       <c r="J28" s="34" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="K28" s="34"/>
     </row>
@@ -1496,7 +1568,7 @@
     </row>
     <row r="31" ht="21" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="33" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="B31" s="33"/>
       <c r="C31" s="33"/>
@@ -1507,7 +1579,7 @@
       <c r="H31" s="33"/>
       <c r="I31" s="33"/>
       <c r="J31" s="40" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="K31" s="40"/>
     </row>
@@ -1552,7 +1624,7 @@
     </row>
     <row r="35" ht="21" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="33" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="B35" s="33"/>
       <c r="C35" s="33"/>
@@ -1563,7 +1635,7 @@
       <c r="H35" s="33"/>
       <c r="I35" s="33"/>
       <c r="J35" s="40" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="K35" s="40"/>
     </row>
@@ -1596,46 +1668,46 @@
     </row>
     <row r="38" ht="24" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="43" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="B38" s="44" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="C38" s="44" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="D38" s="44"/>
       <c r="E38" s="44" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="F38" s="44"/>
       <c r="G38" s="44" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="H38" s="44"/>
       <c r="I38" s="44"/>
       <c r="J38" s="45" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="K38" s="45"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="46"/>
       <c r="B39" s="47" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="C39" s="47" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="D39" s="47"/>
       <c r="E39" s="47"/>
       <c r="F39" s="47" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="G39" s="47"/>
       <c r="H39" s="47"/>
       <c r="I39" s="34" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="J39" s="34"/>
       <c r="K39" s="34"/>
@@ -1655,7 +1727,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="49" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="B41" s="49"/>
       <c r="C41" s="49"/>
@@ -1664,13 +1736,13 @@
       <c r="F41" s="49"/>
       <c r="G41" s="49"/>
       <c r="H41" s="47" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="K41" s="50"/>
     </row>
     <row r="42" ht="15" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="51" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B42" s="51"/>
       <c r="C42" s="51"/>
@@ -1685,7 +1757,7 @@
     </row>
     <row r="43" ht="18.75" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="52" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="B43" s="52"/>
       <c r="C43" s="52"/>

</xml_diff>

<commit_message>
Antes de migrar al sistema v2
</commit_message>
<xml_diff>
--- a/newAdmision.xlsx
+++ b/newAdmision.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="78">
   <si>
     <t xml:space="preserve">HOSPITAL GENERAL SAN JUAN DE DIOS </t>
   </si>
@@ -40,19 +40,19 @@
     <t>No. Expediente Clinico</t>
   </si>
   <si>
-    <t>CRUZ</t>
-  </si>
-  <si>
-    <t>PALACIOS</t>
-  </si>
-  <si>
-    <t>THELMA</t>
-  </si>
-  <si>
-    <t>NOHEMI</t>
-  </si>
-  <si>
-    <t>17-406 CAD</t>
+    <t>ALVAREZ</t>
+  </si>
+  <si>
+    <t>MEDA</t>
+  </si>
+  <si>
+    <t>CLAUDIA</t>
+  </si>
+  <si>
+    <t>ELIZBETH</t>
+  </si>
+  <si>
+    <t>17-8077</t>
   </si>
   <si>
     <t xml:space="preserve">Dirección actual </t>
@@ -70,18 +70,15 @@
     <t>Teléfono</t>
   </si>
   <si>
-    <t>24 AV. 19-35 ZONA 6</t>
-  </si>
-  <si>
-    <t>BARRIO SAN ANTONIO</t>
+    <t/>
+  </si>
+  <si>
+    <t>3RA CALLE A LOTE 23 ZONA 7 CUIDAD PERONIA</t>
   </si>
   <si>
     <t>GUATEMALA</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t xml:space="preserve">Dirección habitual </t>
   </si>
   <si>
@@ -100,13 +97,10 @@
     <t>Sexo</t>
   </si>
   <si>
-    <t>13/11/1967</t>
-  </si>
-  <si>
-    <t>49 AÑOS</t>
-  </si>
-  <si>
-    <t>LOS AMATES IZABAL</t>
+    <t>1987-04-06</t>
+  </si>
+  <si>
+    <t>29</t>
   </si>
   <si>
     <t>FEMENINO</t>
@@ -124,7 +118,7 @@
     <t>No. De Cédula</t>
   </si>
   <si>
-    <t>Soltero</t>
+    <t>Casado</t>
   </si>
   <si>
     <t>AMA DE CASA</t>
@@ -133,7 +127,7 @@
     <t>GUATEMALTECA</t>
   </si>
   <si>
-    <t>3665331851805</t>
+    <t>2291340330101</t>
   </si>
   <si>
     <t>Nombre del Cónyugue</t>
@@ -142,16 +136,16 @@
     <t xml:space="preserve">Dirección si difiere a la indicada </t>
   </si>
   <si>
+    <t>MIGUEL AJANEL</t>
+  </si>
+  <si>
     <t>Nombre del Padre:</t>
   </si>
   <si>
     <t xml:space="preserve">Nombre de la Madre: </t>
   </si>
   <si>
-    <t>VICTOR CRUZ</t>
-  </si>
-  <si>
-    <t>JESÚS PALACIOS</t>
+    <t>DORIAN ALVAREZ</t>
   </si>
   <si>
     <t>En caso de emergencia notificar a :</t>
@@ -163,13 +157,7 @@
     <t>Dirección</t>
   </si>
   <si>
-    <t>VICKY CRUZ</t>
-  </si>
-  <si>
-    <t>HIJA</t>
-  </si>
-  <si>
-    <t>3407-4086</t>
+    <t>ESPOSO</t>
   </si>
   <si>
     <t xml:space="preserve">Otras Hospitalizaciones </t>
@@ -196,13 +184,13 @@
     <t>Dias de estancia</t>
   </si>
   <si>
-    <t>18/10/2017</t>
-  </si>
-  <si>
-    <t>08:15</t>
-  </si>
-  <si>
-    <t>CL. 31</t>
+    <t>2017-10-19</t>
+  </si>
+  <si>
+    <t>14:20</t>
+  </si>
+  <si>
+    <t>L Y P</t>
   </si>
   <si>
     <t xml:space="preserve">IMPRESIÓN CLINICA DE INGRESO </t>
@@ -1154,13 +1142,13 @@
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1177,91 +1165,91 @@
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K9" s="10"/>
     </row>
     <row r="10" ht="18" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I11" s="12"/>
       <c r="J11" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K11" s="10"/>
     </row>
     <row r="12" ht="14.25" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="13" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="I12" s="13"/>
       <c r="J12" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
@@ -1269,20 +1257,20 @@
     </row>
     <row r="14" ht="21.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G14" s="13"/>
       <c r="H14" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
@@ -1290,14 +1278,14 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
@@ -1307,14 +1295,14 @@
     </row>
     <row r="16" ht="12" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
@@ -1324,14 +1312,14 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
       <c r="F17" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
@@ -1341,14 +1329,14 @@
     </row>
     <row r="18" ht="16.5" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
       <c r="F18" s="22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
@@ -1358,18 +1346,18 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G19" s="24"/>
       <c r="H19" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I19" s="24"/>
       <c r="J19" s="9" t="s">
@@ -1379,35 +1367,35 @@
     </row>
     <row r="20" ht="17.25" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I20" s="13"/>
       <c r="J20" s="7" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="K20" s="7"/>
     </row>
     <row r="21" ht="12.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="25" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G21" s="25"/>
       <c r="H21" s="25"/>
@@ -1417,14 +1405,14 @@
     </row>
     <row r="22" ht="12.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -1434,39 +1422,39 @@
     </row>
     <row r="23" ht="18" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="28" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D23" s="28" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E23" s="28"/>
       <c r="F23" s="18" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G23" s="29"/>
       <c r="H23" s="30" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I23" s="30"/>
       <c r="J23" s="31" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="K23" s="31"/>
     </row>
     <row r="24" ht="16.5" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="13"/>
@@ -1478,7 +1466,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="32" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
@@ -1519,7 +1507,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B28" s="33"/>
       <c r="C28" s="33"/>
@@ -1530,7 +1518,7 @@
       <c r="H28" s="33"/>
       <c r="I28" s="33"/>
       <c r="J28" s="34" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="K28" s="34"/>
     </row>
@@ -1562,7 +1550,7 @@
     </row>
     <row r="31" ht="21" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="33" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B31" s="33"/>
       <c r="C31" s="33"/>
@@ -1573,7 +1561,7 @@
       <c r="H31" s="33"/>
       <c r="I31" s="33"/>
       <c r="J31" s="40" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="K31" s="40"/>
     </row>
@@ -1618,7 +1606,7 @@
     </row>
     <row r="35" ht="21" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B35" s="33"/>
       <c r="C35" s="33"/>
@@ -1629,7 +1617,7 @@
       <c r="H35" s="33"/>
       <c r="I35" s="33"/>
       <c r="J35" s="40" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="K35" s="40"/>
     </row>
@@ -1662,46 +1650,46 @@
     </row>
     <row r="38" ht="24" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="43" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B38" s="44" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C38" s="44" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D38" s="44"/>
       <c r="E38" s="44" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F38" s="44"/>
       <c r="G38" s="44" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H38" s="44"/>
       <c r="I38" s="44"/>
       <c r="J38" s="45" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K38" s="45"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="46"/>
       <c r="B39" s="47" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C39" s="47" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D39" s="47"/>
       <c r="E39" s="47"/>
       <c r="F39" s="47" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G39" s="47"/>
       <c r="H39" s="47"/>
       <c r="I39" s="34" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J39" s="34"/>
       <c r="K39" s="34"/>
@@ -1721,7 +1709,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="49" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B41" s="49"/>
       <c r="C41" s="49"/>
@@ -1730,13 +1718,13 @@
       <c r="F41" s="49"/>
       <c r="G41" s="49"/>
       <c r="H41" s="47" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="K41" s="50"/>
     </row>
     <row r="42" ht="15" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="51" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B42" s="51"/>
       <c r="C42" s="51"/>
@@ -1751,7 +1739,7 @@
     </row>
     <row r="43" ht="18.75" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="52" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B43" s="52"/>
       <c r="C43" s="52"/>

</xml_diff>

<commit_message>
Version 2 funcionando un fin de semana completo sin errores
</commit_message>
<xml_diff>
--- a/newAdmision.xlsx
+++ b/newAdmision.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="81">
   <si>
     <t xml:space="preserve">HOSPITAL GENERAL SAN JUAN DE DIOS </t>
   </si>
@@ -40,19 +40,19 @@
     <t>No. Expediente Clinico</t>
   </si>
   <si>
-    <t>ALVAREZ</t>
-  </si>
-  <si>
-    <t>MEDA</t>
-  </si>
-  <si>
-    <t>CLAUDIA</t>
-  </si>
-  <si>
-    <t>ELIZBETH</t>
-  </si>
-  <si>
-    <t>17-8077</t>
+    <t>Cac</t>
+  </si>
+  <si>
+    <t>Ac</t>
+  </si>
+  <si>
+    <t>Delci</t>
+  </si>
+  <si>
+    <t>Celestina Romelia</t>
+  </si>
+  <si>
+    <t>2017-0020967</t>
   </si>
   <si>
     <t xml:space="preserve">Dirección actual </t>
@@ -70,13 +70,16 @@
     <t>Teléfono</t>
   </si>
   <si>
+    <t>Aldea Tameja</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>3RA CALLE A LOTE 23 ZONA 7 CUIDAD PERONIA</t>
-  </si>
-  <si>
-    <t>GUATEMALA</t>
+    <t>Livingston</t>
+  </si>
+  <si>
+    <t>Izabal</t>
   </si>
   <si>
     <t xml:space="preserve">Dirección habitual </t>
@@ -97,10 +100,13 @@
     <t>Sexo</t>
   </si>
   <si>
-    <t>1987-04-06</t>
-  </si>
-  <si>
-    <t>29</t>
+    <t>2007-03-11</t>
+  </si>
+  <si>
+    <t>10 años</t>
+  </si>
+  <si>
+    <t>Livingston, Izabal</t>
   </si>
   <si>
     <t>FEMENINO</t>
@@ -118,16 +124,13 @@
     <t>No. De Cédula</t>
   </si>
   <si>
-    <t>Casado</t>
-  </si>
-  <si>
-    <t>AMA DE CASA</t>
-  </si>
-  <si>
-    <t>GUATEMALTECA</t>
-  </si>
-  <si>
-    <t>2291340330101</t>
+    <t>Soltero</t>
+  </si>
+  <si>
+    <t>Estudiante</t>
+  </si>
+  <si>
+    <t>Guatemalteca</t>
   </si>
   <si>
     <t>Nombre del Cónyugue</t>
@@ -136,16 +139,16 @@
     <t xml:space="preserve">Dirección si difiere a la indicada </t>
   </si>
   <si>
-    <t>MIGUEL AJANEL</t>
-  </si>
-  <si>
     <t>Nombre del Padre:</t>
   </si>
   <si>
     <t xml:space="preserve">Nombre de la Madre: </t>
   </si>
   <si>
-    <t>DORIAN ALVAREZ</t>
+    <t>Nicolas Cac Cxac</t>
+  </si>
+  <si>
+    <t>Clara Ac Caal</t>
   </si>
   <si>
     <t>En caso de emergencia notificar a :</t>
@@ -157,7 +160,13 @@
     <t>Dirección</t>
   </si>
   <si>
-    <t>ESPOSO</t>
+    <t>Nicolas Cac</t>
+  </si>
+  <si>
+    <t>Padre</t>
+  </si>
+  <si>
+    <t>45230310</t>
   </si>
   <si>
     <t xml:space="preserve">Otras Hospitalizaciones </t>
@@ -184,13 +193,13 @@
     <t>Dias de estancia</t>
   </si>
   <si>
-    <t>2017-10-19</t>
-  </si>
-  <si>
-    <t>14:20</t>
-  </si>
-  <si>
-    <t>L Y P</t>
+    <t>2017-10-16</t>
+  </si>
+  <si>
+    <t>11:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hemato. pedia. </t>
   </si>
   <si>
     <t xml:space="preserve">IMPRESIÓN CLINICA DE INGRESO </t>
@@ -1138,17 +1147,17 @@
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1165,91 +1174,91 @@
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K9" s="10"/>
     </row>
     <row r="10" ht="18" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I11" s="12"/>
       <c r="J11" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K11" s="10"/>
     </row>
     <row r="12" ht="14.25" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="13" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="I12" s="13"/>
       <c r="J12" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
@@ -1257,20 +1266,20 @@
     </row>
     <row r="14" ht="21.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G14" s="13"/>
       <c r="H14" s="7" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
@@ -1278,14 +1287,14 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
@@ -1295,14 +1304,14 @@
     </row>
     <row r="16" ht="12" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
@@ -1329,14 +1338,14 @@
     </row>
     <row r="18" ht="16.5" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
       <c r="F18" s="22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
@@ -1346,18 +1355,18 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="24" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G19" s="24"/>
       <c r="H19" s="24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I19" s="24"/>
       <c r="J19" s="9" t="s">
@@ -1367,35 +1376,35 @@
     </row>
     <row r="20" ht="17.25" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I20" s="13"/>
       <c r="J20" s="7" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="K20" s="7"/>
     </row>
     <row r="21" ht="12.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="25" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G21" s="25"/>
       <c r="H21" s="25"/>
@@ -1405,14 +1414,14 @@
     </row>
     <row r="22" ht="12.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -1422,39 +1431,39 @@
     </row>
     <row r="23" ht="18" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="28" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D23" s="28" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E23" s="28"/>
       <c r="F23" s="18" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G23" s="29"/>
       <c r="H23" s="30" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="I23" s="30"/>
       <c r="J23" s="31" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="K23" s="31"/>
     </row>
     <row r="24" ht="16.5" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="13"/>
@@ -1466,7 +1475,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="32" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
@@ -1507,7 +1516,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B28" s="33"/>
       <c r="C28" s="33"/>
@@ -1518,7 +1527,7 @@
       <c r="H28" s="33"/>
       <c r="I28" s="33"/>
       <c r="J28" s="34" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="K28" s="34"/>
     </row>
@@ -1550,7 +1559,7 @@
     </row>
     <row r="31" ht="21" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="33" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B31" s="33"/>
       <c r="C31" s="33"/>
@@ -1561,7 +1570,7 @@
       <c r="H31" s="33"/>
       <c r="I31" s="33"/>
       <c r="J31" s="40" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="K31" s="40"/>
     </row>
@@ -1606,7 +1615,7 @@
     </row>
     <row r="35" ht="21" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="33" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B35" s="33"/>
       <c r="C35" s="33"/>
@@ -1617,7 +1626,7 @@
       <c r="H35" s="33"/>
       <c r="I35" s="33"/>
       <c r="J35" s="40" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="K35" s="40"/>
     </row>
@@ -1650,46 +1659,46 @@
     </row>
     <row r="38" ht="24" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="43" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B38" s="44" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C38" s="44" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D38" s="44"/>
       <c r="E38" s="44" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F38" s="44"/>
       <c r="G38" s="44" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="H38" s="44"/>
       <c r="I38" s="44"/>
       <c r="J38" s="45" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="K38" s="45"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="46"/>
       <c r="B39" s="47" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C39" s="47" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D39" s="47"/>
       <c r="E39" s="47"/>
       <c r="F39" s="47" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G39" s="47"/>
       <c r="H39" s="47"/>
       <c r="I39" s="34" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="J39" s="34"/>
       <c r="K39" s="34"/>
@@ -1709,7 +1718,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="49" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B41" s="49"/>
       <c r="C41" s="49"/>
@@ -1718,13 +1727,13 @@
       <c r="F41" s="49"/>
       <c r="G41" s="49"/>
       <c r="H41" s="47" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K41" s="50"/>
     </row>
     <row r="42" ht="15" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="51" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B42" s="51"/>
       <c r="C42" s="51"/>
@@ -1739,7 +1748,7 @@
     </row>
     <row r="43" ht="18.75" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="52" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B43" s="52"/>
       <c r="C43" s="52"/>

</xml_diff>